<commit_message>
added albums loading and post history
</commit_message>
<xml_diff>
--- a/30_Meiring.xlsx
+++ b/30_Meiring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\IMY220_Project_Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4BE8F0-7837-4180-BD03-34CB4106D402}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B67EE7-A9B5-412A-80A6-AED9F15FEF14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BC8E386B-9B68-4E1C-A935-933319C6EB34}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="155">
   <si>
     <t xml:space="preserve">Position_Surname: </t>
   </si>
@@ -1125,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{956CF17A-F085-48B4-B2E7-798B312D3D72}">
   <dimension ref="A1:D186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="94" zoomScaleNormal="94" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="94" zoomScaleNormal="94" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1350,21 +1350,27 @@
       <c r="A41" t="s">
         <v>25</v>
       </c>
-      <c r="B41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="C41" s="8"/>
     </row>
     <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>99</v>
       </c>
-      <c r="B42" s="1"/>
+      <c r="B42" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="C42" s="8"/>
     </row>
     <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>26</v>
       </c>
-      <c r="B43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="C43" s="8"/>
     </row>
     <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1530,7 +1536,9 @@
       <c r="A71" t="s">
         <v>41</v>
       </c>
-      <c r="B71" s="1"/>
+      <c r="B71" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="C71" s="8"/>
     </row>
     <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1624,14 +1632,18 @@
       <c r="A87" t="s">
         <v>140</v>
       </c>
-      <c r="B87" s="1"/>
+      <c r="B87" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="C87" s="8"/>
     </row>
     <row r="88" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>109</v>
       </c>
-      <c r="B88" s="1"/>
+      <c r="B88" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="C88" s="8"/>
     </row>
     <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1652,14 +1664,18 @@
       <c r="A91" t="s">
         <v>139</v>
       </c>
-      <c r="B91" s="1"/>
+      <c r="B91" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="C91" s="8"/>
     </row>
     <row r="92" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>112</v>
       </c>
-      <c r="B92" s="1"/>
+      <c r="B92" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="C92" s="8"/>
     </row>
     <row r="93" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1680,7 +1696,9 @@
       <c r="A95" t="s">
         <v>115</v>
       </c>
-      <c r="B95" s="1"/>
+      <c r="B95" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="C95" s="8"/>
     </row>
     <row r="96" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>